<commit_message>
Add two more sonarCloud diaries
</commit_message>
<xml_diff>
--- a/SonarCloud/IT79_2018_StosicKristijan_DnevnikProjekta.xlsx
+++ b/SonarCloud/IT79_2018_StosicKristijan_DnevnikProjekta.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Fakultet\4.Godina\7.Semestar\Upravljanje razvojem informacionih sistema\Projekat\tim-7---auctionland\SonarCloud\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INZENJERSTO INFORMACIONIH SISTEMA\2021-2022\VII SEMESTAR\Upravljanje razvojem informacionih sistema\Projekat\Mikroservisi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F78727E-9E74-4566-95FA-EFE417D85A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF1BEE8-C425-4BF0-806B-B9BCCEAE846C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21240" windowHeight="15390" xr2:uid="{20C5DEC2-B10F-44F9-9ED1-5DB010ECB74B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{20C5DEC2-B10F-44F9-9ED1-5DB010ECB74B}"/>
   </bookViews>
   <sheets>
     <sheet name="Diary" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="64">
   <si>
     <t>Upravljanje razvojem informacionih sistema</t>
   </si>
@@ -367,7 +367,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,8 +399,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF777777"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
-      <color theme="1"/>
+      <color rgb="FF777777"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -437,7 +444,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -770,19 +777,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -816,11 +810,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -848,11 +847,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1170,8 +1164,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,88 +1184,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="26"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="29"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="29"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="32"/>
     </row>
     <row r="4" spans="1:12" ht="57.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="21" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1279,7 +1273,7 @@
       <c r="A5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -1317,7 +1311,7 @@
       <c r="A6" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -1355,7 +1349,7 @@
       <c r="A7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -1393,7 +1387,7 @@
       <c r="A8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1431,7 +1425,7 @@
       <c r="A9" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C9" s="10" t="s">
@@ -1469,7 +1463,7 @@
       <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -1507,7 +1501,7 @@
       <c r="A11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="22" t="s">
         <v>50</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -1545,7 +1539,7 @@
       <c r="A12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="23" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="10" t="s">
@@ -1583,7 +1577,7 @@
       <c r="A13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="23" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -1621,7 +1615,7 @@
       <c r="A14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="23" t="s">
         <v>55</v>
       </c>
       <c r="C14" s="10" t="s">
@@ -1659,7 +1653,7 @@
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="23" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="10" t="s">
@@ -1697,7 +1691,7 @@
       <c r="A16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -1735,7 +1729,7 @@
       <c r="A17" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -1773,7 +1767,7 @@
       <c r="A18" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C18" s="10" t="s">
@@ -1811,7 +1805,7 @@
       <c r="A19" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -1849,7 +1843,7 @@
       <c r="A20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -1887,7 +1881,7 @@
       <c r="A21" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="10" t="s">
@@ -1925,7 +1919,7 @@
       <c r="A22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="22" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="10" t="s">
@@ -1963,7 +1957,7 @@
       <c r="A23" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="23" t="s">
         <v>61</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -2001,7 +1995,7 @@
       <c r="A24" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="23" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="10" t="s">
@@ -2036,18 +2030,42 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="13"/>
+      <c r="A25" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="16">
+        <v>1</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
@@ -15738,19 +15756,19 @@
           <x14:formula1>
             <xm:f>Codes!$G$13:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>K14 J5:J1000 K24</xm:sqref>
+          <xm:sqref>K14 K24:K25 J5:J1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77E0D190-3C56-4952-9EB8-961170AA1D70}">
           <x14:formula1>
             <xm:f>Codes!$B$21:$B$25</xm:f>
           </x14:formula1>
-          <xm:sqref>K5:K13 K15:K23 K25:K1000</xm:sqref>
+          <xm:sqref>K5:K13 K15:K23 K26:K1000</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{08384ABE-884A-494F-97C5-F3EC37D9F7EC}">
           <x14:formula1>
             <xm:f>Codes!$G$26:$G$27</xm:f>
           </x14:formula1>
-          <xm:sqref>L5:L19 L22 L24</xm:sqref>
+          <xm:sqref>L5:L19 L22 L24:L25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>